<commit_message>
Sửa lỗi anotation và hoàn thành form thêm hóa đơn đổi trả
</commit_message>
<xml_diff>
--- a/Reports/ref-Các quy định.xlsx
+++ b/Reports/ref-Các quy định.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\Đồ án kì 1-2015\OOAD-2015\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\OOAD-2015\trunk\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7305"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Quy định đổi, trả" sheetId="1" r:id="rId1"/>
@@ -414,6 +414,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -423,32 +444,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -768,7 +768,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="15"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
@@ -777,7 +777,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="15"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="15"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
@@ -795,7 +795,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="16"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
@@ -804,7 +804,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="15"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
@@ -824,7 +824,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="15"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
@@ -833,7 +833,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="15"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
@@ -842,7 +842,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="16"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
@@ -851,25 +851,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="20"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="15"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="16"/>
-      <c r="F15" s="17" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -943,16 +943,16 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="11"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="20"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">

</xml_diff>